<commit_message>
add: godunov not working
</commit_message>
<xml_diff>
--- a/Lax_Friedrichs_method/results/error norms/lax_friedrichs_shock_wave.xlsx
+++ b/Lax_Friedrichs_method/results/error norms/lax_friedrichs_shock_wave.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gas_dyn\Lax_Friedrichs_method\results\error norms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gas_dyn\idk\Lax_Friedrichs_method\results\error norms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EA6AF8E-D928-448F-80E2-A8DA6A005C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7A5F10-358D-4867-8769-2A273A70C9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1044" yWindow="1536" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="first_half_of_grid" sheetId="2" r:id="rId1"/>
-    <sheet name="whole_grid" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="first_half_of_grid" sheetId="2" r:id="rId2"/>
+    <sheet name="whole_grid" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="12">
   <si>
     <t>100</t>
   </si>
@@ -66,9 +67,6 @@
   </si>
   <si>
     <t>uniform</t>
-  </si>
-  <si>
-    <t>rho1 = p1 = 1.0, u1 = 1.8520259177, rho2 = 0.125, p2 = 0.1, u2 = 0; lax-friedrichs; courant = 0.5; time = 0.2</t>
   </si>
 </sst>
 </file>
@@ -125,6 +123,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304305</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>45120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Рисунок 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BD59249-F93E-4EFD-8914-EF9674AFF060}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3961905" cy="4800000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -411,11 +458,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C2" sqref="C2:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,477 +485,472 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>12</v>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>7.1616266726340959E-3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4.5918713605149401E-5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1.0618643831935119E-14</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3.301359828204346E-15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>4.2927452385586023E-3</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1">
-        <v>9.0806172981563292E-7</v>
+        <f>C2/D2</f>
+        <v>155.96313812743611</v>
       </c>
       <c r="E3" s="1">
-        <v>1.0618643831935119E-14</v>
+        <f>D2/E2</f>
+        <v>4324348224.8694344</v>
       </c>
       <c r="F3" s="1">
-        <v>3.301359828204346E-15</v>
+        <f>E2/F2</f>
+        <v>3.2164454602062396</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5.4122905695097642E-3</v>
+      </c>
       <c r="D4" s="1">
-        <f>C3/D3</f>
-        <v>4727.3716065868939</v>
+        <v>3.2802343453578297E-5</v>
       </c>
       <c r="E4" s="1">
-        <f>D3/E3</f>
-        <v>85515791.299513772</v>
+        <v>5.2775682025544214E-15</v>
       </c>
       <c r="F4" s="1">
-        <f>E3/F3</f>
-        <v>3.2164454602062396</v>
+        <v>1.696941518368994E-15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1">
-        <v>3.088833599257003E-3</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1">
-        <v>6.4861670532925839E-7</v>
+        <f>C4/D4</f>
+        <v>164.99707032118633</v>
       </c>
       <c r="E5" s="1">
-        <v>5.2775682025544214E-15</v>
+        <f>D4/E4</f>
+        <v>6215427673.2419062</v>
       </c>
       <c r="F5" s="1">
-        <v>1.696941518368994E-15</v>
+        <f>E4/F4</f>
+        <v>3.1100471910351555</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6.1018789365867203E-3</v>
+      </c>
       <c r="D6" s="1">
-        <f>C5/D5</f>
-        <v>4762.1863172472767</v>
+        <v>3.8813881224384509E-5</v>
       </c>
       <c r="E6" s="1">
-        <f>D5/E5</f>
-        <v>122900677.06094603</v>
+        <v>7.4250314814751395E-15</v>
       </c>
       <c r="F6" s="1">
-        <f>E5/F5</f>
-        <v>3.1100471910351555</v>
+        <v>2.315059029554221E-15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3.645057535006237E-3</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1">
-        <v>7.6745430202139319E-7</v>
+        <f>C6/D6</f>
+        <v>157.20867751698236</v>
       </c>
       <c r="E7" s="1">
-        <v>7.4250314814751395E-15</v>
+        <f>D6/E6</f>
+        <v>5227436586.7972469</v>
       </c>
       <c r="F7" s="1">
-        <v>2.315059029554221E-15</v>
+        <f>E6/F6</f>
+        <v>3.2072752299991572</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5.0640347845460197E-2</v>
+      </c>
       <c r="D8" s="1">
-        <f>C7/D7</f>
-        <v>4749.5434261108994</v>
+        <v>1.0267736506045851E-3</v>
       </c>
       <c r="E8" s="1">
-        <f>D7/E7</f>
-        <v>103360410.51625577</v>
+        <v>7.5085150605660295E-13</v>
       </c>
       <c r="F8" s="1">
-        <f>E7/F7</f>
-        <v>3.2072752299991572</v>
+        <v>7.3820649940519458E-13</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3.035429268091051E-2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C9" s="1"/>
       <c r="D9" s="1">
-        <v>2.0304877556338029E-5</v>
+        <f>C8/D8</f>
+        <v>49.31987475101463</v>
       </c>
       <c r="E9" s="1">
-        <v>7.5085150605660295E-13</v>
+        <f>D8/E8</f>
+        <v>1367478978.6293399</v>
       </c>
       <c r="F9" s="1">
-        <v>7.3820649940519458E-13</v>
+        <f>E8/F8</f>
+        <v>1.0171293623960194</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3.8270673634523557E-2</v>
+      </c>
       <c r="D10" s="1">
-        <f>C9/D9</f>
-        <v>1494.9261622824031</v>
+        <v>7.3348269783496292E-4</v>
       </c>
       <c r="E10" s="1">
-        <f>D9/E9</f>
-        <v>27042467.641807389</v>
+        <v>3.7318042642007299E-13</v>
       </c>
       <c r="F10" s="1">
-        <f>E9/F9</f>
-        <v>1.0171293623960194</v>
+        <v>3.7944765889147802E-13</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2.1841351839914779E-2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C11" s="1"/>
       <c r="D11" s="1">
-        <v>1.4503510444581721E-5</v>
+        <f>C10/D10</f>
+        <v>52.176654946991867</v>
       </c>
       <c r="E11" s="1">
-        <v>3.7318042642007299E-13</v>
+        <f>D10/E10</f>
+        <v>1965490807.9485211</v>
       </c>
       <c r="F11" s="1">
-        <v>3.7944765889147802E-13</v>
+        <f>E10/F10</f>
+        <v>0.98348327542798875</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4.3146799740398291E-2</v>
+      </c>
       <c r="D12" s="1">
-        <f>C11/D11</f>
-        <v>1505.935540459059</v>
+        <v>8.679047688832654E-4</v>
       </c>
       <c r="E12" s="1">
-        <f>D11/E11</f>
-        <v>38864606.548939809</v>
+        <v>5.2502901110746685E-13</v>
       </c>
       <c r="F12" s="1">
-        <f>E11/F11</f>
-        <v>0.98348327542798875</v>
+        <v>5.1766293620079321E-13</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2.5774449008180319E-2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="1">
-        <v>1.7160799889444891E-5</v>
+        <f>C12/D12</f>
+        <v>49.713748889656813</v>
       </c>
       <c r="E13" s="1">
-        <v>5.2502901110746685E-13</v>
+        <f>D12/E12</f>
+        <v>1653060593.8375778</v>
       </c>
       <c r="F13" s="1">
-        <v>5.1766293620079321E-13</v>
+        <f>E12/F12</f>
+        <v>1.0142294809837737</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.3877696398247969E-3</v>
+      </c>
       <c r="D14" s="1">
-        <f>C13/D13</f>
-        <v>1501.9375072390089</v>
+        <v>3.916944883216256E-6</v>
       </c>
       <c r="E14" s="1">
-        <f>D13/E13</f>
-        <v>32685431.712138835</v>
+        <v>8.5782492220687349E-16</v>
       </c>
       <c r="F14" s="1">
-        <f>E13/F13</f>
-        <v>1.0142294809837737</v>
+        <v>1.8395951428829001E-16</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1">
-        <v>9.5525469430877475E-4</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1">
-        <v>8.1280641145653476E-8</v>
+        <f>C14/D14</f>
+        <v>354.29899608014927</v>
       </c>
       <c r="E15" s="1">
-        <v>8.5782492220687349E-16</v>
+        <f>D14/E14</f>
+        <v>4566135561.9505348</v>
       </c>
       <c r="F15" s="1">
-        <v>1.8395951428829001E-16</v>
+        <f>E14/F14</f>
+        <v>4.6631179992274996</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.0379567523444121E-3</v>
+      </c>
       <c r="D16" s="1">
-        <f>C15/D15</f>
-        <v>11752.548710792957</v>
+        <v>2.7980322221223818E-6</v>
       </c>
       <c r="E16" s="1">
-        <f>D15/E15</f>
-        <v>94752016.45639737</v>
+        <v>3.7601033398004802E-16</v>
       </c>
       <c r="F16" s="1">
-        <f>E15/F15</f>
-        <v>4.6631179992274996</v>
+        <v>3.8000713686869861E-17</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="1">
-        <v>6.8639676836558918E-4</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1">
-        <v>5.8057681392886813E-8</v>
+        <f>C16/D16</f>
+        <v>370.95954225898595</v>
       </c>
       <c r="E17" s="1">
-        <v>3.7601033398004802E-16</v>
+        <f>D16/E16</f>
+        <v>7441370540.2864056</v>
       </c>
       <c r="F17" s="1">
-        <v>3.8000713686869861E-17</v>
+        <f>E16/F16</f>
+        <v>9.8948229519691466</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.1802282530690329E-3</v>
+      </c>
       <c r="D18" s="1">
-        <f>C17/D17</f>
-        <v>11822.669316065489</v>
+        <v>3.3107788361399489E-6</v>
       </c>
       <c r="E18" s="1">
-        <f>D17/E17</f>
-        <v>154404483.45754105</v>
+        <v>6.3746785627927243E-16</v>
       </c>
       <c r="F18" s="1">
-        <f>E17/F17</f>
-        <v>9.8948229519691466</v>
+        <v>1.624500534092022E-16</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="1">
-        <v>8.1032805016668875E-4</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1">
-        <v>6.8694819539416587E-8</v>
+        <f>C18/D18</f>
+        <v>356.48054777499607</v>
       </c>
       <c r="E19" s="1">
-        <v>6.3746785627927243E-16</v>
+        <f>D18/E18</f>
+        <v>5193640437.7533169</v>
       </c>
       <c r="F19" s="1">
-        <v>1.624500534092022E-16</v>
+        <f>E18/F18</f>
+        <v>3.9240852366698098</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3.2412247600915323E-2</v>
+      </c>
       <c r="D20" s="1">
-        <f>C19/D19</f>
-        <v>11796.057629960414</v>
+        <v>5.0974651935475901E-4</v>
       </c>
       <c r="E20" s="1">
-        <f>D19/E19</f>
-        <v>107762013.19446863</v>
+        <v>1.117994585797533E-13</v>
       </c>
       <c r="F20" s="1">
-        <f>E19/F19</f>
-        <v>3.9240852366698098</v>
+        <v>1.101341240428155E-13</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1.539738685284109E-2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="1">
-        <v>9.7654235502453446E-6</v>
+        <f>C20/D20</f>
+        <v>63.585029755461576</v>
       </c>
       <c r="E21" s="1">
-        <v>1.117994585797533E-13</v>
+        <f>D20/E20</f>
+        <v>4559472164.0903654</v>
       </c>
       <c r="F21" s="1">
-        <v>1.101341240428155E-13</v>
+        <f>E20/F20</f>
+        <v>1.0151209677419362</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2.4885157362210971E-2</v>
+      </c>
       <c r="D22" s="1">
-        <f>C21/D21</f>
-        <v>1576.7249391301875</v>
+        <v>3.6415591156568888E-4</v>
       </c>
       <c r="E22" s="1">
-        <f>D21/E21</f>
-        <v>87347681.950347543</v>
+        <v>5.5067062021407758E-14</v>
       </c>
       <c r="F22" s="1">
-        <f>E21/F21</f>
-        <v>1.0151209677419362</v>
+        <v>5.6621374255882977E-14</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1.1098256916271421E-2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1">
-        <v>6.975320852919964E-6</v>
+        <f>C22/D22</f>
+        <v>68.336546440279378</v>
       </c>
       <c r="E23" s="1">
-        <v>5.5067062021407758E-14</v>
+        <f>D22/E22</f>
+        <v>6612953337.2258062</v>
       </c>
       <c r="F23" s="1">
-        <v>5.6621374255882977E-14</v>
+        <f>E22/F22</f>
+        <v>0.97254901960784312</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2.7700327321930951E-2</v>
+      </c>
       <c r="D24" s="1">
-        <f>C23/D23</f>
-        <v>1591.0747548803492</v>
+        <v>4.3090255263589228E-4</v>
       </c>
       <c r="E24" s="1">
-        <f>D23/E23</f>
-        <v>126669566.10483873</v>
+        <v>7.7049477908985864E-14</v>
       </c>
       <c r="F24" s="1">
-        <f>E23/F23</f>
-        <v>0.97254901960784312</v>
+        <v>7.638334409421077E-14</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1.3090928952779191E-2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1">
-        <v>8.2533216643199125E-6</v>
+        <f>C24/D24</f>
+        <v>64.284435430897545</v>
       </c>
       <c r="E25" s="1">
-        <v>7.7049477908985864E-14</v>
+        <f>D24/E24</f>
+        <v>5592543445.1988468</v>
       </c>
       <c r="F25" s="1">
-        <v>7.638334409421077E-14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1">
-        <f>C25/D25</f>
-        <v>1586.1406455745966</v>
-      </c>
-      <c r="E26" s="1">
-        <f>D25/E25</f>
-        <v>107117165.33717579</v>
-      </c>
-      <c r="F26" s="1">
-        <f>E25/F25</f>
+        <f>E24/F24</f>
         <v>1.0087209302325582</v>
       </c>
     </row>
@@ -905,12 +960,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -940,16 +995,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>8.0607742968607024E-2</v>
+        <v>8.1846555505187157E-2</v>
       </c>
       <c r="D2" s="1">
-        <v>2.778422075170096E-2</v>
+        <v>2.7328864596910411E-2</v>
       </c>
       <c r="E2" s="1">
-        <v>9.2602665437818907E-3</v>
+        <v>9.240907386716856E-3</v>
       </c>
       <c r="F2" s="1">
-        <v>2.7774598687146769E-3</v>
+        <v>2.7540107987645271E-3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -959,15 +1014,15 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1">
         <f>C2/D2</f>
-        <v>2.9012058207057034</v>
+        <v>2.9948758103342534</v>
       </c>
       <c r="E3" s="1">
         <f>D2/E2</f>
-        <v>3.0003694408081141</v>
+        <v>2.957378908070619</v>
       </c>
       <c r="F3" s="1">
         <f>E2/F2</f>
-        <v>3.3340775318086799</v>
+        <v>3.3554361482033426</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -978,16 +1033,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1">
-        <v>6.9376385764684495E-2</v>
+        <v>6.3409993735565079E-2</v>
       </c>
       <c r="D4" s="1">
-        <v>3.990115073039098E-2</v>
+        <v>3.4302126248465743E-2</v>
       </c>
       <c r="E4" s="1">
-        <v>2.1538732143200321E-2</v>
+        <v>1.8319580446567469E-2</v>
       </c>
       <c r="F4" s="1">
-        <v>1.186874210963855E-2</v>
+        <v>1.001507052250445E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -997,15 +1052,15 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <f>C4/D4</f>
-        <v>1.7387063905363387</v>
+        <v>1.8485732714134964</v>
       </c>
       <c r="E5" s="1">
         <f>D4/E4</f>
-        <v>1.8525301519656805</v>
+        <v>1.8724296851947237</v>
       </c>
       <c r="F5" s="1">
         <f>E4/F4</f>
-        <v>1.8147443043445031</v>
+        <v>1.829201342656779</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1016,16 +1071,16 @@
         <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>0.20513988728244911</v>
+        <v>0.29756697682764949</v>
       </c>
       <c r="D6" s="1">
-        <v>6.5985799288093464E-2</v>
+        <v>9.3561276807603955E-2</v>
       </c>
       <c r="E6" s="1">
-        <v>2.113511859447036E-2</v>
+        <v>2.9693712735441111E-2</v>
       </c>
       <c r="F6" s="1">
-        <v>6.6121841002574318E-3</v>
+        <v>9.151793979708292E-3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1035,15 +1090,15 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <f>C6/D6</f>
-        <v>3.1088490174501038</v>
+        <v>3.1804501496869855</v>
       </c>
       <c r="E7" s="1">
         <f>D6/E6</f>
-        <v>3.1220926910416065</v>
+        <v>3.1508783573545291</v>
       </c>
       <c r="F7" s="1">
         <f>E6/F6</f>
-        <v>3.1963899180676938</v>
+        <v>3.2445783636824812</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1054,16 +1109,16 @@
         <v>5</v>
       </c>
       <c r="C8" s="1">
-        <v>0.80607742968607021</v>
+        <v>0.81846555505187157</v>
       </c>
       <c r="D8" s="1">
-        <v>0.8786142058829064</v>
+        <v>0.86421457992576312</v>
       </c>
       <c r="E8" s="1">
-        <v>0.9260266543781891</v>
+        <v>0.92409073867168567</v>
       </c>
       <c r="F8" s="1">
-        <v>0.87830992948506237</v>
+        <v>0.87089468247955382</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1073,15 +1128,15 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1">
         <f>C8/D8</f>
-        <v>0.91744183543681146</v>
+        <v>0.94706288699986818</v>
       </c>
       <c r="E9" s="1">
         <f>D8/E8</f>
-        <v>0.94880012549193915</v>
+        <v>0.93520532536448719</v>
       </c>
       <c r="F9" s="1">
         <f>E8/F8</f>
-        <v>1.0543278896107917</v>
+        <v>1.0610820771584866</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1092,16 +1147,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="1">
-        <v>0.69376385764684501</v>
+        <v>0.63409993735565084</v>
       </c>
       <c r="D10" s="1">
-        <v>1.261785175697266</v>
+        <v>1.084728475317986</v>
       </c>
       <c r="E10" s="1">
-        <v>2.1538732143200319</v>
+        <v>1.8319580446567469</v>
       </c>
       <c r="F10" s="1">
-        <v>3.753225802760972</v>
+        <v>3.1670433778326692</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1111,15 +1166,15 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1">
         <f>C10/D10</f>
-        <v>0.54982723763850627</v>
+        <v>0.58457019593752779</v>
       </c>
       <c r="E11" s="1">
         <f>D10/E10</f>
-        <v>0.58582147143494046</v>
+        <v>0.59211425637273862</v>
       </c>
       <c r="F11" s="1">
         <f>E10/F10</f>
-        <v>0.5738725372546426</v>
+        <v>0.57844425418335355</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1130,16 +1185,16 @@
         <v>8</v>
       </c>
       <c r="C12" s="1">
-        <v>2.0513988728244912</v>
+        <v>2.9756697682764952</v>
       </c>
       <c r="D12" s="1">
-        <v>2.086654189770925</v>
+        <v>2.9586673550551592</v>
       </c>
       <c r="E12" s="1">
-        <v>2.113511859447037</v>
+        <v>2.9693712735441111</v>
       </c>
       <c r="F12" s="1">
-        <v>2.0909562065164629</v>
+        <v>2.8940513652495001</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1149,15 +1204,15 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1">
         <f>C12/D12</f>
-        <v>0.98310437967188791</v>
+        <v>1.0057466457634332</v>
       </c>
       <c r="E13" s="1">
         <f>D12/E12</f>
-        <v>0.98729239698558457</v>
+        <v>0.99639522393702684</v>
       </c>
       <c r="F13" s="1">
         <f>E12/F12</f>
-        <v>1.010787243109291</v>
+        <v>1.0260257676138784</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1168,16 +1223,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="1">
-        <v>2.5926892236975529E-2</v>
+        <v>3.451720011855737E-2</v>
       </c>
       <c r="D14" s="1">
-        <v>5.8654366612529056E-3</v>
+        <v>5.7778379519405013E-3</v>
       </c>
       <c r="E14" s="1">
-        <v>1.291360229748883E-3</v>
+        <v>1.141024817491862E-3</v>
       </c>
       <c r="F14" s="1">
-        <v>2.3824292506024569E-4</v>
+        <v>2.1261753055885931E-4</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1187,15 +1242,15 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1">
         <f>C14/D14</f>
-        <v>4.4202833879783698</v>
+        <v>5.9740685712662955</v>
       </c>
       <c r="E15" s="1">
         <f>D14/E14</f>
-        <v>4.5420607868599872</v>
+        <v>5.0637268036299394</v>
       </c>
       <c r="F15" s="1">
         <f>E14/F14</f>
-        <v>5.4203508012770163</v>
+        <v>5.366560388942105</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1206,16 +1261,16 @@
         <v>7</v>
       </c>
       <c r="C16" s="1">
-        <v>3.651835542302069E-2</v>
+        <v>3.1757137587193812E-2</v>
       </c>
       <c r="D16" s="1">
-        <v>1.5016687535543201E-2</v>
+        <v>1.131223865480576E-2</v>
       </c>
       <c r="E16" s="1">
-        <v>4.4698957954995757E-3</v>
+        <v>3.2833282894834731E-3</v>
       </c>
       <c r="F16" s="1">
-        <v>1.296547928634339E-3</v>
+        <v>9.4514764944816226E-4</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1225,15 +1280,15 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1">
         <f>C16/D16</f>
-        <v>2.4318515875478464</v>
+        <v>2.8073256369730566</v>
       </c>
       <c r="E17" s="1">
         <f>D16/E16</f>
-        <v>3.3595162443523736</v>
+        <v>3.4453571673106684</v>
       </c>
       <c r="F17" s="1">
         <f>E16/F16</f>
-        <v>3.4475361047452688</v>
+        <v>3.4738787018097019</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1244,16 +1299,16 @@
         <v>8</v>
       </c>
       <c r="C18" s="1">
-        <v>3.6077391344923812E-2</v>
+        <v>9.5039548230615251E-2</v>
       </c>
       <c r="D18" s="1">
-        <v>6.8512881657917116E-3</v>
+        <v>1.177539310068575E-2</v>
       </c>
       <c r="E18" s="1">
-        <v>1.3466138574153E-3</v>
+        <v>1.701192412025185E-3</v>
       </c>
       <c r="F18" s="1">
-        <v>2.3566050094437439E-4</v>
+        <v>2.6013985163225191E-4</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1263,15 +1318,15 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1">
         <f>C18/D18</f>
-        <v>5.2657822108632368</v>
+        <v>8.0710297667328437</v>
       </c>
       <c r="E19" s="1">
         <f>D18/E18</f>
-        <v>5.0877897387318747</v>
+        <v>6.9218467102540915</v>
       </c>
       <c r="F19" s="1">
         <f>E18/F18</f>
-        <v>5.7142111300746006</v>
+        <v>6.5395301848256793</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1282,16 +1337,16 @@
         <v>5</v>
       </c>
       <c r="C20" s="1">
-        <v>0.71426158550574004</v>
+        <v>0.41783239788303939</v>
       </c>
       <c r="D20" s="1">
-        <v>0.71426158550574004</v>
+        <v>0.41831333198961068</v>
       </c>
       <c r="E20" s="1">
-        <v>0.71426158550574004</v>
+        <v>0.47401745583459209</v>
       </c>
       <c r="F20" s="1">
-        <v>0.71426158550574004</v>
+        <v>0.40361626857155197</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1301,15 +1356,15 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1">
         <f>C20/D20</f>
-        <v>1</v>
+        <v>0.99885030174801304</v>
       </c>
       <c r="E21" s="1">
         <f>D20/E20</f>
-        <v>1</v>
+        <v>0.8824850790633767</v>
       </c>
       <c r="F21" s="1">
         <f>E20/F20</f>
-        <v>1</v>
+        <v>1.1744260396445334</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1320,16 +1375,16 @@
         <v>7</v>
       </c>
       <c r="C22" s="1">
-        <v>0.31565128793443831</v>
+        <v>0.222842307440801</v>
       </c>
       <c r="D22" s="1">
-        <v>0.31565128793443831</v>
+        <v>0.20427119971944349</v>
       </c>
       <c r="E22" s="1">
-        <v>0.31565128793443831</v>
+        <v>0.22054456590923391</v>
       </c>
       <c r="F22" s="1">
-        <v>0.31565128793443831</v>
+        <v>0.21087823016189691</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1339,15 +1394,15 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1">
         <f>C22/D22</f>
-        <v>1</v>
+        <v>1.0909139797820937</v>
       </c>
       <c r="E23" s="1">
         <f>D22/E22</f>
-        <v>1</v>
+        <v>0.92621279911068954</v>
       </c>
       <c r="F23" s="1">
         <f>E22/F22</f>
-        <v>1</v>
+        <v>1.0458384715193971</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1358,16 +1413,16 @@
         <v>8</v>
       </c>
       <c r="C24" s="1">
-        <v>2.023158858530647</v>
+        <v>1.54096625715114</v>
       </c>
       <c r="D24" s="1">
-        <v>2.023158858530647</v>
+        <v>1.517200405291667</v>
       </c>
       <c r="E24" s="1">
-        <v>2.023158858530647</v>
+        <v>1.629680009882279</v>
       </c>
       <c r="F24" s="1">
-        <v>2.023158858530647</v>
+        <v>1.4867528789645601</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1377,15 +1432,15 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1">
         <f>C24/D24</f>
-        <v>1</v>
+        <v>1.0156642799307085</v>
       </c>
       <c r="E25" s="1">
         <f>D24/E24</f>
-        <v>1</v>
+        <v>0.93098055820250436</v>
       </c>
       <c r="F25" s="1">
         <f>E24/F24</f>
-        <v>1</v>
+        <v>1.0961337509009967</v>
       </c>
     </row>
   </sheetData>

</xml_diff>